<commit_message>
Some positive change And Good Result by SnapPrice dfd
</commit_message>
<xml_diff>
--- a/i_60m.xlsx
+++ b/i_60m.xlsx
@@ -48881,10 +48881,20 @@
       <c r="I1361" t="n">
         <v>0.274</v>
       </c>
-      <c r="J1361" t="inlineStr"/>
-      <c r="K1361" t="inlineStr"/>
-      <c r="L1361" t="inlineStr"/>
-      <c r="M1361" t="inlineStr"/>
+      <c r="J1361" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K1361" t="n">
+        <v>0.7168866395950317</v>
+      </c>
+      <c r="L1361" t="n">
+        <v>1019.846859962344</v>
+      </c>
+      <c r="M1361" t="n">
+        <v>0</v>
+      </c>
       <c r="N1361" t="n">
         <v>8.355</v>
       </c>
@@ -48924,12 +48934,8 @@
       <c r="K1362" t="inlineStr"/>
       <c r="L1362" t="inlineStr"/>
       <c r="M1362" t="inlineStr"/>
-      <c r="N1362" t="n">
-        <v>8.868</v>
-      </c>
-      <c r="O1362" t="n">
-        <v>2.556</v>
-      </c>
+      <c r="N1362" t="inlineStr"/>
+      <c r="O1362" t="inlineStr"/>
     </row>
     <row r="1363">
       <c r="A1363" s="2" t="n">
@@ -48963,12 +48969,8 @@
       <c r="K1363" t="inlineStr"/>
       <c r="L1363" t="inlineStr"/>
       <c r="M1363" t="inlineStr"/>
-      <c r="N1363" t="n">
-        <v>9.034000000000001</v>
-      </c>
-      <c r="O1363" t="n">
-        <v>2.743</v>
-      </c>
+      <c r="N1363" t="inlineStr"/>
+      <c r="O1363" t="inlineStr"/>
     </row>
     <row r="1364">
       <c r="A1364" s="2" t="n">
@@ -49002,12 +49004,8 @@
       <c r="K1364" t="inlineStr"/>
       <c r="L1364" t="inlineStr"/>
       <c r="M1364" t="inlineStr"/>
-      <c r="N1364" t="n">
-        <v>9.231999999999999</v>
-      </c>
-      <c r="O1364" t="n">
-        <v>2.966</v>
-      </c>
+      <c r="N1364" t="inlineStr"/>
+      <c r="O1364" t="inlineStr"/>
     </row>
     <row r="1365">
       <c r="A1365" s="2" t="n">
@@ -49041,12 +49039,8 @@
       <c r="K1365" t="inlineStr"/>
       <c r="L1365" t="inlineStr"/>
       <c r="M1365" t="inlineStr"/>
-      <c r="N1365" t="n">
-        <v>9.936</v>
-      </c>
-      <c r="O1365" t="n">
-        <v>3.767</v>
-      </c>
+      <c r="N1365" t="inlineStr"/>
+      <c r="O1365" t="inlineStr"/>
     </row>
     <row r="1366">
       <c r="A1366" s="2" t="n">
@@ -49080,12 +49074,8 @@
       <c r="K1366" t="inlineStr"/>
       <c r="L1366" t="inlineStr"/>
       <c r="M1366" t="inlineStr"/>
-      <c r="N1366" t="n">
-        <v>9.688000000000001</v>
-      </c>
-      <c r="O1366" t="n">
-        <v>3.484</v>
-      </c>
+      <c r="N1366" t="inlineStr"/>
+      <c r="O1366" t="inlineStr"/>
     </row>
     <row r="1367">
       <c r="A1367" s="2" t="n">
@@ -49119,12 +49109,8 @@
       <c r="K1367" t="inlineStr"/>
       <c r="L1367" t="inlineStr"/>
       <c r="M1367" t="inlineStr"/>
-      <c r="N1367" t="n">
-        <v>10.371</v>
-      </c>
-      <c r="O1367" t="n">
-        <v>4.268</v>
-      </c>
+      <c r="N1367" t="inlineStr"/>
+      <c r="O1367" t="inlineStr"/>
     </row>
     <row r="1368">
       <c r="A1368" s="2" t="n">
@@ -49158,12 +49144,8 @@
       <c r="K1368" t="inlineStr"/>
       <c r="L1368" t="inlineStr"/>
       <c r="M1368" t="inlineStr"/>
-      <c r="N1368" t="n">
-        <v>10.047</v>
-      </c>
-      <c r="O1368" t="n">
-        <v>3.894</v>
-      </c>
+      <c r="N1368" t="inlineStr"/>
+      <c r="O1368" t="inlineStr"/>
     </row>
     <row r="1369">
       <c r="A1369" s="2" t="n">
@@ -49197,12 +49179,8 @@
       <c r="K1369" t="inlineStr"/>
       <c r="L1369" t="inlineStr"/>
       <c r="M1369" t="inlineStr"/>
-      <c r="N1369" t="n">
-        <v>10.45</v>
-      </c>
-      <c r="O1369" t="n">
-        <v>4.359</v>
-      </c>
+      <c r="N1369" t="inlineStr"/>
+      <c r="O1369" t="inlineStr"/>
     </row>
     <row r="1370">
       <c r="A1370" s="2" t="n">
@@ -49236,12 +49214,8 @@
       <c r="K1370" t="inlineStr"/>
       <c r="L1370" t="inlineStr"/>
       <c r="M1370" t="inlineStr"/>
-      <c r="N1370" t="n">
-        <v>12.141</v>
-      </c>
-      <c r="O1370" t="n">
-        <v>6.359</v>
-      </c>
+      <c r="N1370" t="inlineStr"/>
+      <c r="O1370" t="inlineStr"/>
     </row>
     <row r="1371">
       <c r="A1371" s="2" t="n">
@@ -49275,12 +49249,8 @@
       <c r="K1371" t="inlineStr"/>
       <c r="L1371" t="inlineStr"/>
       <c r="M1371" t="inlineStr"/>
-      <c r="N1371" t="n">
-        <v>12.257</v>
-      </c>
-      <c r="O1371" t="n">
-        <v>6.499</v>
-      </c>
+      <c r="N1371" t="inlineStr"/>
+      <c r="O1371" t="inlineStr"/>
     </row>
     <row r="1372">
       <c r="A1372" s="2" t="n">
@@ -49314,12 +49284,8 @@
       <c r="K1372" t="inlineStr"/>
       <c r="L1372" t="inlineStr"/>
       <c r="M1372" t="inlineStr"/>
-      <c r="N1372" t="n">
-        <v>11.424</v>
-      </c>
-      <c r="O1372" t="n">
-        <v>5.502</v>
-      </c>
+      <c r="N1372" t="inlineStr"/>
+      <c r="O1372" t="inlineStr"/>
     </row>
     <row r="1373">
       <c r="A1373" s="2" t="n">
@@ -49353,12 +49319,8 @@
       <c r="K1373" t="inlineStr"/>
       <c r="L1373" t="inlineStr"/>
       <c r="M1373" t="inlineStr"/>
-      <c r="N1373" t="n">
-        <v>11.037</v>
-      </c>
-      <c r="O1373" t="n">
-        <v>5.046</v>
-      </c>
+      <c r="N1373" t="inlineStr"/>
+      <c r="O1373" t="inlineStr"/>
     </row>
     <row r="1374">
       <c r="A1374" s="2" t="n">
@@ -49392,12 +49354,8 @@
       <c r="K1374" t="inlineStr"/>
       <c r="L1374" t="inlineStr"/>
       <c r="M1374" t="inlineStr"/>
-      <c r="N1374" t="n">
-        <v>10.524</v>
-      </c>
-      <c r="O1374" t="n">
-        <v>4.446</v>
-      </c>
+      <c r="N1374" t="inlineStr"/>
+      <c r="O1374" t="inlineStr"/>
     </row>
     <row r="1375">
       <c r="A1375" s="2" t="n">
@@ -49431,12 +49389,8 @@
       <c r="K1375" t="inlineStr"/>
       <c r="L1375" t="inlineStr"/>
       <c r="M1375" t="inlineStr"/>
-      <c r="N1375" t="n">
-        <v>9.114000000000001</v>
-      </c>
-      <c r="O1375" t="n">
-        <v>2.833</v>
-      </c>
+      <c r="N1375" t="inlineStr"/>
+      <c r="O1375" t="inlineStr"/>
     </row>
     <row r="1376">
       <c r="A1376" s="2" t="n">
@@ -49470,12 +49424,8 @@
       <c r="K1376" t="inlineStr"/>
       <c r="L1376" t="inlineStr"/>
       <c r="M1376" t="inlineStr"/>
-      <c r="N1376" t="n">
-        <v>9.247999999999999</v>
-      </c>
-      <c r="O1376" t="n">
-        <v>2.983</v>
-      </c>
+      <c r="N1376" t="inlineStr"/>
+      <c r="O1376" t="inlineStr"/>
     </row>
     <row r="1377">
       <c r="A1377" s="2" t="n">
@@ -49509,12 +49459,8 @@
       <c r="K1377" t="inlineStr"/>
       <c r="L1377" t="inlineStr"/>
       <c r="M1377" t="inlineStr"/>
-      <c r="N1377" t="n">
-        <v>10.809</v>
-      </c>
-      <c r="O1377" t="n">
-        <v>4.777</v>
-      </c>
+      <c r="N1377" t="inlineStr"/>
+      <c r="O1377" t="inlineStr"/>
     </row>
     <row r="1378">
       <c r="A1378" s="2" t="n">
@@ -49548,12 +49494,8 @@
       <c r="K1378" t="inlineStr"/>
       <c r="L1378" t="inlineStr"/>
       <c r="M1378" t="inlineStr"/>
-      <c r="N1378" t="n">
-        <v>10.52</v>
-      </c>
-      <c r="O1378" t="n">
-        <v>4.441</v>
-      </c>
+      <c r="N1378" t="inlineStr"/>
+      <c r="O1378" t="inlineStr"/>
     </row>
     <row r="1379">
       <c r="A1379" s="2" t="n">
@@ -49587,12 +49529,8 @@
       <c r="K1379" t="inlineStr"/>
       <c r="L1379" t="inlineStr"/>
       <c r="M1379" t="inlineStr"/>
-      <c r="N1379" t="n">
-        <v>10.519</v>
-      </c>
-      <c r="O1379" t="n">
-        <v>4.439</v>
-      </c>
+      <c r="N1379" t="inlineStr"/>
+      <c r="O1379" t="inlineStr"/>
     </row>
     <row r="1380">
       <c r="A1380" s="2" t="n">
@@ -49626,12 +49564,8 @@
       <c r="K1380" t="inlineStr"/>
       <c r="L1380" t="inlineStr"/>
       <c r="M1380" t="inlineStr"/>
-      <c r="N1380" t="n">
-        <v>10.544</v>
-      </c>
-      <c r="O1380" t="n">
-        <v>4.469</v>
-      </c>
+      <c r="N1380" t="inlineStr"/>
+      <c r="O1380" t="inlineStr"/>
     </row>
     <row r="1381">
       <c r="A1381" s="2" t="n">
@@ -49665,12 +49599,8 @@
       <c r="K1381" t="inlineStr"/>
       <c r="L1381" t="inlineStr"/>
       <c r="M1381" t="inlineStr"/>
-      <c r="N1381" t="n">
-        <v>10.981</v>
-      </c>
-      <c r="O1381" t="n">
-        <v>4.979</v>
-      </c>
+      <c r="N1381" t="inlineStr"/>
+      <c r="O1381" t="inlineStr"/>
     </row>
     <row r="1382">
       <c r="A1382" s="2" t="n">
@@ -49704,12 +49634,8 @@
       <c r="K1382" t="inlineStr"/>
       <c r="L1382" t="inlineStr"/>
       <c r="M1382" t="inlineStr"/>
-      <c r="N1382" t="n">
-        <v>10.229</v>
-      </c>
-      <c r="O1382" t="n">
-        <v>4.105</v>
-      </c>
+      <c r="N1382" t="inlineStr"/>
+      <c r="O1382" t="inlineStr"/>
     </row>
     <row r="1383">
       <c r="A1383" s="2" t="n">
@@ -49743,12 +49669,8 @@
       <c r="K1383" t="inlineStr"/>
       <c r="L1383" t="inlineStr"/>
       <c r="M1383" t="inlineStr"/>
-      <c r="N1383" t="n">
-        <v>10.608</v>
-      </c>
-      <c r="O1383" t="n">
-        <v>4.543</v>
-      </c>
+      <c r="N1383" t="inlineStr"/>
+      <c r="O1383" t="inlineStr"/>
     </row>
     <row r="1384">
       <c r="A1384" s="2" t="n">
@@ -49782,12 +49704,8 @@
       <c r="K1384" t="inlineStr"/>
       <c r="L1384" t="inlineStr"/>
       <c r="M1384" t="inlineStr"/>
-      <c r="N1384" t="n">
-        <v>11.108</v>
-      </c>
-      <c r="O1384" t="n">
-        <v>5.129</v>
-      </c>
+      <c r="N1384" t="inlineStr"/>
+      <c r="O1384" t="inlineStr"/>
     </row>
     <row r="1385">
       <c r="A1385" s="2" t="n">
@@ -49821,12 +49739,8 @@
       <c r="K1385" t="inlineStr"/>
       <c r="L1385" t="inlineStr"/>
       <c r="M1385" t="inlineStr"/>
-      <c r="N1385" t="n">
-        <v>11.937</v>
-      </c>
-      <c r="O1385" t="n">
-        <v>6.114</v>
-      </c>
+      <c r="N1385" t="inlineStr"/>
+      <c r="O1385" t="inlineStr"/>
     </row>
     <row r="1386">
       <c r="A1386" s="2" t="n">
@@ -49860,12 +49774,8 @@
       <c r="K1386" t="inlineStr"/>
       <c r="L1386" t="inlineStr"/>
       <c r="M1386" t="inlineStr"/>
-      <c r="N1386" t="n">
-        <v>11.259</v>
-      </c>
-      <c r="O1386" t="n">
-        <v>5.307</v>
-      </c>
+      <c r="N1386" t="inlineStr"/>
+      <c r="O1386" t="inlineStr"/>
     </row>
     <row r="1387">
       <c r="A1387" s="2" t="n">
@@ -49899,12 +49809,8 @@
       <c r="K1387" t="inlineStr"/>
       <c r="L1387" t="inlineStr"/>
       <c r="M1387" t="inlineStr"/>
-      <c r="N1387" t="n">
-        <v>12.024</v>
-      </c>
-      <c r="O1387" t="n">
-        <v>6.218</v>
-      </c>
+      <c r="N1387" t="inlineStr"/>
+      <c r="O1387" t="inlineStr"/>
     </row>
     <row r="1388">
       <c r="A1388" s="2" t="n">
@@ -49938,12 +49844,8 @@
       <c r="K1388" t="inlineStr"/>
       <c r="L1388" t="inlineStr"/>
       <c r="M1388" t="inlineStr"/>
-      <c r="N1388" t="n">
-        <v>12.878</v>
-      </c>
-      <c r="O1388" t="n">
-        <v>7.255</v>
-      </c>
+      <c r="N1388" t="inlineStr"/>
+      <c r="O1388" t="inlineStr"/>
     </row>
     <row r="1389">
       <c r="A1389" s="2" t="n">
@@ -49977,12 +49879,8 @@
       <c r="K1389" t="inlineStr"/>
       <c r="L1389" t="inlineStr"/>
       <c r="M1389" t="inlineStr"/>
-      <c r="N1389" t="n">
-        <v>12.811</v>
-      </c>
-      <c r="O1389" t="n">
-        <v>7.173</v>
-      </c>
+      <c r="N1389" t="inlineStr"/>
+      <c r="O1389" t="inlineStr"/>
     </row>
     <row r="1390">
       <c r="A1390" s="2" t="n">
@@ -50016,12 +49914,8 @@
       <c r="K1390" t="inlineStr"/>
       <c r="L1390" t="inlineStr"/>
       <c r="M1390" t="inlineStr"/>
-      <c r="N1390" t="n">
-        <v>12.156</v>
-      </c>
-      <c r="O1390" t="n">
-        <v>6.377</v>
-      </c>
+      <c r="N1390" t="inlineStr"/>
+      <c r="O1390" t="inlineStr"/>
     </row>
     <row r="1391">
       <c r="A1391" s="2" t="n">
@@ -50055,12 +49949,8 @@
       <c r="K1391" t="inlineStr"/>
       <c r="L1391" t="inlineStr"/>
       <c r="M1391" t="inlineStr"/>
-      <c r="N1391" t="n">
-        <v>12.055</v>
-      </c>
-      <c r="O1391" t="n">
-        <v>6.255</v>
-      </c>
+      <c r="N1391" t="inlineStr"/>
+      <c r="O1391" t="inlineStr"/>
     </row>
     <row r="1392">
       <c r="A1392" s="2" t="n">
@@ -50094,12 +49984,8 @@
       <c r="K1392" t="inlineStr"/>
       <c r="L1392" t="inlineStr"/>
       <c r="M1392" t="inlineStr"/>
-      <c r="N1392" t="n">
-        <v>11.668</v>
-      </c>
-      <c r="O1392" t="n">
-        <v>5.792</v>
-      </c>
+      <c r="N1392" t="inlineStr"/>
+      <c r="O1392" t="inlineStr"/>
     </row>
     <row r="1393">
       <c r="A1393" s="2" t="n">
@@ -50133,12 +50019,8 @@
       <c r="K1393" t="inlineStr"/>
       <c r="L1393" t="inlineStr"/>
       <c r="M1393" t="inlineStr"/>
-      <c r="N1393" t="n">
-        <v>11.78</v>
-      </c>
-      <c r="O1393" t="n">
-        <v>5.926</v>
-      </c>
+      <c r="N1393" t="inlineStr"/>
+      <c r="O1393" t="inlineStr"/>
     </row>
     <row r="1394">
       <c r="A1394" s="2" t="n">
@@ -50172,12 +50054,8 @@
       <c r="K1394" t="inlineStr"/>
       <c r="L1394" t="inlineStr"/>
       <c r="M1394" t="inlineStr"/>
-      <c r="N1394" t="n">
-        <v>12.233</v>
-      </c>
-      <c r="O1394" t="n">
-        <v>6.47</v>
-      </c>
+      <c r="N1394" t="inlineStr"/>
+      <c r="O1394" t="inlineStr"/>
     </row>
     <row r="1395">
       <c r="A1395" s="2" t="n">
@@ -50211,12 +50089,8 @@
       <c r="K1395" t="inlineStr"/>
       <c r="L1395" t="inlineStr"/>
       <c r="M1395" t="inlineStr"/>
-      <c r="N1395" t="n">
-        <v>11.726</v>
-      </c>
-      <c r="O1395" t="n">
-        <v>5.862</v>
-      </c>
+      <c r="N1395" t="inlineStr"/>
+      <c r="O1395" t="inlineStr"/>
     </row>
     <row r="1396">
       <c r="A1396" s="2" t="n">
@@ -50250,12 +50124,8 @@
       <c r="K1396" t="inlineStr"/>
       <c r="L1396" t="inlineStr"/>
       <c r="M1396" t="inlineStr"/>
-      <c r="N1396" t="n">
-        <v>11.05</v>
-      </c>
-      <c r="O1396" t="n">
-        <v>5.06</v>
-      </c>
+      <c r="N1396" t="inlineStr"/>
+      <c r="O1396" t="inlineStr"/>
     </row>
     <row r="1397">
       <c r="A1397" s="2" t="n">
@@ -50289,12 +50159,8 @@
       <c r="K1397" t="inlineStr"/>
       <c r="L1397" t="inlineStr"/>
       <c r="M1397" t="inlineStr"/>
-      <c r="N1397" t="n">
-        <v>11.134</v>
-      </c>
-      <c r="O1397" t="n">
-        <v>5.159</v>
-      </c>
+      <c r="N1397" t="inlineStr"/>
+      <c r="O1397" t="inlineStr"/>
     </row>
     <row r="1398">
       <c r="A1398" s="2" t="n">
@@ -50328,12 +50194,8 @@
       <c r="K1398" t="inlineStr"/>
       <c r="L1398" t="inlineStr"/>
       <c r="M1398" t="inlineStr"/>
-      <c r="N1398" t="n">
-        <v>11.049</v>
-      </c>
-      <c r="O1398" t="n">
-        <v>5.06</v>
-      </c>
+      <c r="N1398" t="inlineStr"/>
+      <c r="O1398" t="inlineStr"/>
     </row>
     <row r="1399">
       <c r="A1399" s="2" t="n">
@@ -50367,12 +50229,8 @@
       <c r="K1399" t="inlineStr"/>
       <c r="L1399" t="inlineStr"/>
       <c r="M1399" t="inlineStr"/>
-      <c r="N1399" t="n">
-        <v>10.506</v>
-      </c>
-      <c r="O1399" t="n">
-        <v>4.425</v>
-      </c>
+      <c r="N1399" t="inlineStr"/>
+      <c r="O1399" t="inlineStr"/>
     </row>
     <row r="1400">
       <c r="A1400" s="2" t="n">
@@ -50406,12 +50264,8 @@
       <c r="K1400" t="inlineStr"/>
       <c r="L1400" t="inlineStr"/>
       <c r="M1400" t="inlineStr"/>
-      <c r="N1400" t="n">
-        <v>10.752</v>
-      </c>
-      <c r="O1400" t="n">
-        <v>4.712</v>
-      </c>
+      <c r="N1400" t="inlineStr"/>
+      <c r="O1400" t="inlineStr"/>
     </row>
     <row r="1401">
       <c r="A1401" s="2" t="n">
@@ -50441,26 +50295,12 @@
       <c r="I1401" t="n">
         <v>-0.498</v>
       </c>
-      <c r="J1401" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="K1401" t="n">
-        <v>0.7325010895729065</v>
-      </c>
-      <c r="L1401" t="n">
-        <v>1041.955125469267</v>
-      </c>
-      <c r="M1401" t="n">
-        <v>0</v>
-      </c>
-      <c r="N1401" t="n">
-        <v>10.308</v>
-      </c>
-      <c r="O1401" t="n">
-        <v>4.196</v>
-      </c>
+      <c r="J1401" t="inlineStr"/>
+      <c r="K1401" t="inlineStr"/>
+      <c r="L1401" t="inlineStr"/>
+      <c r="M1401" t="inlineStr"/>
+      <c r="N1401" t="inlineStr"/>
+      <c r="O1401" t="inlineStr"/>
     </row>
     <row r="1402">
       <c r="A1402" s="2" t="n">
@@ -56592,28 +56432,28 @@
         <v>45366.625</v>
       </c>
       <c r="B1577" t="n">
-        <v>0.7192511558532715</v>
+        <v>0.7184900045394897</v>
       </c>
       <c r="C1577" t="n">
-        <v>44.732</v>
+        <v>44.43</v>
       </c>
       <c r="D1577" t="n">
-        <v>40.8234670830578</v>
+        <v>40.76855799214871</v>
       </c>
       <c r="E1577" t="n">
-        <v>0.7144991199175517</v>
+        <v>0.7144483764966328</v>
       </c>
       <c r="F1577" t="n">
         <v>0.736</v>
       </c>
       <c r="G1577" t="n">
-        <v>0.661</v>
+        <v>0.5629999999999999</v>
       </c>
       <c r="H1577" t="n">
-        <v>-2.329</v>
+        <v>-2.437</v>
       </c>
       <c r="I1577" t="n">
-        <v>0.574</v>
+        <v>0.469</v>
       </c>
       <c r="J1577" t="inlineStr"/>
       <c r="K1577" t="inlineStr"/>

</xml_diff>